<commit_message>
excel table something wrong
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/飞机大战数据.xlsx
+++ b/ExcelTool/bin/table/飞机大战数据.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E511B88-1B6F-49FA-9B63-232F3BFB3B28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9235FFF8-9184-4B82-B6F5-6CB2A062DE7B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5808" yWindow="3492" windowWidth="21600" windowHeight="10452" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>int</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -229,6 +229,10 @@
   </si>
   <si>
     <t>5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -399,25 +403,25 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -426,7 +430,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -437,10 +441,10 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -862,7 +866,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -892,6 +896,9 @@
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>